<commit_message>
vault backup: 2024-09-08 19:22:02
</commit_message>
<xml_diff>
--- a/2024-2/Notas.xlsx
+++ b/2024-2/Notas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UNIVERSIDAD\2024\2do Semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248B2750-EE55-4518-9FE7-09DD0C71EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46358EF-E47A-4FE2-989F-C0841FAAD107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCD97180-9067-40E7-A2AA-1AE726290FDC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>ALGORITMOS DE RUTEO Y REDES RESILIENTES</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Proyecto Final (30%)</t>
+  </si>
+  <si>
+    <t>Eximición</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,8 +219,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -360,37 +369,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -402,135 +542,145 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -860,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE7B4EE-F9F2-400E-A04E-AEDE20258CF2}">
-  <dimension ref="B1:L30"/>
+  <dimension ref="B1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,90 +1023,90 @@
     <col min="11" max="11" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="42" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="9" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8"/>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="42"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="38">
-        <v>1</v>
-      </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40">
-        <v>1</v>
-      </c>
-      <c r="E5" s="40">
-        <v>1</v>
-      </c>
-      <c r="F5" s="40">
-        <v>1</v>
-      </c>
-      <c r="G5" s="40">
-        <v>1</v>
-      </c>
-      <c r="H5" s="40">
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="40">
+        <v>1</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="48">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5" s="47">
         <f>0.7*H5+0.3*B5</f>
         <v>1</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -968,7 +1118,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -980,79 +1130,79 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="str">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="str">
         <f>UPPER("Comunicaciones por luz visible para industrias inteligentes")</f>
         <v>COMUNICACIONES POR LUZ VISIBLE PARA INDUSTRIAS INTELIGENTES</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="42">
-        <v>1</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44">
-        <v>1</v>
-      </c>
-      <c r="E11" s="44">
-        <v>1</v>
-      </c>
-      <c r="F11" s="44">
-        <v>1</v>
-      </c>
-      <c r="G11" s="45">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28">
+        <v>1</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="47">
         <f>0.3*D11+0.4*E11+0.3*F11</f>
         <v>1</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1064,7 +1214,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1076,22 +1226,22 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -1106,72 +1256,80 @@
       <c r="F15" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="46" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="L15" s="55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="34"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="46">
-        <v>1</v>
-      </c>
-      <c r="C17" s="47">
-        <v>1</v>
-      </c>
-      <c r="D17" s="47">
-        <v>1</v>
-      </c>
-      <c r="E17" s="47">
-        <v>1</v>
-      </c>
-      <c r="F17" s="47">
-        <v>1</v>
-      </c>
-      <c r="G17" s="47">
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="56"/>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="48">
         <f>AVERAGE(B17:F17)</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="47">
-        <v>1</v>
-      </c>
-      <c r="I17" s="47">
-        <v>1</v>
-      </c>
-      <c r="J17" s="47">
-        <v>1</v>
-      </c>
-      <c r="K17" s="48">
+        <v>1.86</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="8">
+        <v>1</v>
+      </c>
+      <c r="J17" s="8">
+        <v>1</v>
+      </c>
+      <c r="K17" s="49">
         <f>AVERAGE(G17:J17)</f>
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="L17" s="57" t="str">
+        <f>IF(K17&gt;=5,"SI","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="M17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1183,7 +1341,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1195,207 +1353,195 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
+    <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="27">
-        <v>1</v>
-      </c>
-      <c r="C22" s="28">
-        <v>1</v>
-      </c>
-      <c r="D22" s="28">
-        <v>1</v>
-      </c>
-      <c r="E22" s="28">
-        <v>1</v>
-      </c>
-      <c r="F22" s="28">
-        <v>1</v>
-      </c>
-      <c r="G22" s="28">
-        <v>1</v>
-      </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="1"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="55" t="s">
+        <v>38</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31" t="s">
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29">
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="50">
         <f>0.6*B24+0.4*E24</f>
         <v>1</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="56"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="49">
+    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="53">
         <f>AVERAGE(B22:D22)</f>
         <v>1</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50">
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52">
         <f>AVERAGE(E22:G22)</f>
         <v>1</v>
       </c>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
       <c r="H24" s="51"/>
-      <c r="I24" s="1"/>
+      <c r="I24" s="57" t="str">
+        <f>IF(AND(H23&gt;=5,E24&gt;=4),"SI","NO")</f>
+        <v>NO</v>
+      </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="32" t="str">
+      <c r="K24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="26" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="str">
         <f>UPPER("Sistemas de procesamiento para Big Data")</f>
         <v>SISTEMAS DE PROCESAMIENTO PARA BIG DATA</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36" t="s">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36" t="s">
+      <c r="G28" s="20"/>
+      <c r="H28" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37" t="s">
+      <c r="I28" s="20"/>
+      <c r="J28" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
-    </row>
-    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="52">
-        <v>1</v>
-      </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53">
-        <v>1</v>
-      </c>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53">
-        <v>1</v>
-      </c>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53">
-        <v>1</v>
-      </c>
-      <c r="I30" s="53"/>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11">
+        <v>1</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11">
+        <v>1</v>
+      </c>
+      <c r="I30" s="11"/>
       <c r="J30" s="54">
         <f>B30*0.3+0.1*D30+0.3*F30+0.3*H30</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="D28:E29"/>
-    <mergeCell ref="F28:G29"/>
-    <mergeCell ref="H28:I29"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
+  <mergeCells count="42">
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -1404,13 +1550,46 @@
     <mergeCell ref="B9:C10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="H28:I29"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B5:G5 B11:F11 B17:F17 H17:J17 B22:G22 B30:I30">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:G5 B11:F11 B17:F17 H17:J17 B22:G22 B30:I30">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>"1.1"</formula>
+      <formula>"3.9"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:G5 B11:F11 B17:F17 H17:J17 B22:G22 B30:I30">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>